<commit_message>
updated IG with links to nrces profiles
</commit_message>
<xml_diff>
--- a/v0.7/StructureDefinition-Claim.xlsx
+++ b/v0.7/StructureDefinition-Claim.xlsx
@@ -579,7 +579,7 @@
     <t>Claim.patient</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(Patient)
+    <t xml:space="preserve">Reference(https://nrces.in/ndhm/fhir/r4/StructureDefinition/Patient)
 </t>
   </si>
   <si>
@@ -648,7 +648,7 @@
     <t>Claim.enterer</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(Practitioner|PractitionerRole)
+    <t xml:space="preserve">Reference(https://nrces.in/ndhm/fhir/r4/StructureDefinition/Practitioner|https://nrces.in/ndhm/fhir/r4/StructureDefinition/PractitionerRole)
 </t>
   </si>
   <si>
@@ -667,7 +667,7 @@
     <t>Claim.insurer</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(Organization)
+    <t xml:space="preserve">Reference(https://nrces.in/ndhm/fhir/r4/StructureDefinition/Organization)
 </t>
   </si>
   <si>
@@ -683,7 +683,7 @@
     <t>Claim.provider</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(Practitioner|PractitionerRole|Organization)
+    <t xml:space="preserve">Reference(https://nrces.in/ndhm/fhir/r4/StructureDefinition/Practitioner|https://nrces.in/ndhm/fhir/r4/StructureDefinition/Organization)
 </t>
   </si>
   <si>
@@ -814,7 +814,7 @@
     <t>Claim.related.claim</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(Claim)
+    <t xml:space="preserve">Reference(https://swasth-digital-health-foundation.github.io/standards/v0.7/StructureDefinition-Claim.html)
 </t>
   </si>
   <si>
@@ -939,7 +939,7 @@
     <t>Claim.payee.party</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(Practitioner|PractitionerRole|Organization|Patient|RelatedPerson)
+    <t xml:space="preserve">Reference(https://nrces.in/ndhm/fhir/r4/StructureDefinition/Practitioner|https://nrces.in/ndhm/fhir/r4/StructureDefinition/PractitionerRole|https://nrces.in/ndhm/fhir/r4/StructureDefinition/Organization|https://nrces.in/ndhm/fhir/r4/StructureDefinition/Patient|RelatedPerson)
 </t>
   </si>
   <si>
@@ -1287,7 +1287,7 @@
   </si>
   <si>
     <t>CodeableConcept
-Reference(Condition)</t>
+Reference(https://nrces.in/ndhm/fhir/r4/StructureDefinition/Condition)</t>
   </si>
   <si>
     <t>Nature of illness or problem</t>
@@ -1535,7 +1535,7 @@
     <t>Claim.insurance.coverage</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(Coverage)
+    <t xml:space="preserve">Reference(https://swasth-digital-health-foundation.github.io/standards/v0.7/StructureDefinition-Coverage.html)
 </t>
   </si>
   <si>
@@ -1578,7 +1578,7 @@
     <t>Claim.insurance.claimResponse</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(ClaimResponse)
+    <t xml:space="preserve">Reference(https://swasth-digital-health-foundation.github.io/standards/v0.7/StructureDefinition-ClaimResponse.html)
 </t>
   </si>
   <si>
@@ -1997,7 +1997,7 @@
     <t>Claim.item.encounter</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(Encounter)
+    <t xml:space="preserve">Reference(https://nrces.in/ndhm/fhir/r4/StructureDefinition-Encounter.html)
 </t>
   </si>
   <si>

</xml_diff>